<commit_message>
UPDATE: oscar detail prerpocessing
</commit_message>
<xml_diff>
--- a/predictionsTwo.xlsx
+++ b/predictionsTwo.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CQ51"/>
+  <dimension ref="A1:CO51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,247 +536,247 @@
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>ben wilkins and thomas curley)</t>
+          <t>best actor</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>best actor</t>
+          <t xml:space="preserve">best actor </t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>best actor (matthew mcconaughey)</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>best actress</t>
         </is>
       </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">best actress </t>
+        </is>
+      </c>
       <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>best actress (cate blanchett)</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>best adapted screenplay</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>best animated feature</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>best animated film</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>best art direction</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>best cinematography</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>best director</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>best editing</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>best film editing</t>
         </is>
       </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">best film editing </t>
+        </is>
+      </c>
       <c r="AH1" s="1" t="inlineStr">
         <is>
-          <t>best film editing (tom cross)</t>
+          <t xml:space="preserve">best makeup and hairstyling </t>
         </is>
       </c>
       <c r="AI1" s="1" t="inlineStr">
-        <is>
-          <t>best makeup and hairstyling (adruitha lee and robin mathews)</t>
-        </is>
-      </c>
-      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>best original screenplay</t>
         </is>
       </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">best original screenplay </t>
+        </is>
+      </c>
       <c r="AK1" s="1" t="inlineStr">
-        <is>
-          <t>best original screenplay (spike jonze)</t>
-        </is>
-      </c>
-      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>best original song</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>best picture</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>best sound</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>best sound editing</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>best sound mixing</t>
         </is>
       </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">best sound mixing </t>
+        </is>
+      </c>
       <c r="AQ1" s="1" t="inlineStr">
-        <is>
-          <t>best sound mixing (craig mann</t>
-        </is>
-      </c>
-      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>best supporting actor</t>
         </is>
       </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">best supporting actor </t>
+        </is>
+      </c>
       <c r="AS1" s="1" t="inlineStr">
-        <is>
-          <t>best supporting actor (j.k. simmons)</t>
-        </is>
-      </c>
-      <c r="AT1" s="1" t="inlineStr">
-        <is>
-          <t>best supporting actor (jared leto)</t>
-        </is>
-      </c>
-      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>best supporting actress</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
-          <t>best supporting actress (patricia arquette)</t>
+          <t xml:space="preserve">best supporting actress </t>
         </is>
       </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>best visual effects</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>cinematography</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>costume design</t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>directing</t>
         </is>
       </c>
-      <c r="BA1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>film editing</t>
         </is>
       </c>
-      <c r="BB1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>make up and hair styling</t>
         </is>
       </c>
-      <c r="BC1" s="1" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="BB1" s="1" t="inlineStr">
         <is>
           <t>original song</t>
         </is>
       </c>
-      <c r="BD1" s="1" t="inlineStr">
+      <c r="BC1" s="1" t="inlineStr">
         <is>
           <t>production design</t>
         </is>
       </c>
-      <c r="BE1" s="1" t="inlineStr">
+      <c r="BD1" s="1" t="inlineStr">
         <is>
           <t>sound editing</t>
         </is>
       </c>
-      <c r="BF1" s="1" t="inlineStr">
+      <c r="BE1" s="1" t="inlineStr">
         <is>
           <t>sound mixing</t>
         </is>
       </c>
-      <c r="BG1" s="1" t="inlineStr">
+      <c r="BF1" s="1" t="inlineStr">
         <is>
           <t>visual effects</t>
         </is>
       </c>
+      <c r="BG1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">writing </t>
+        </is>
+      </c>
       <c r="BH1" s="1" t="inlineStr">
         <is>
-          <t>writing (adapted screenplay)</t>
+          <t>drama</t>
         </is>
       </c>
       <c r="BI1" s="1" t="inlineStr">
         <is>
-          <t>writing (original screenplay)</t>
+          <t>action</t>
         </is>
       </c>
       <c r="BJ1" s="1" t="inlineStr">
         <is>
-          <t>sports</t>
+          <t>crime</t>
         </is>
       </c>
       <c r="BK1" s="1" t="inlineStr">
         <is>
-          <t>comedy</t>
+          <t>fantasy</t>
         </is>
       </c>
       <c r="BL1" s="1" t="inlineStr">
         <is>
-          <t>adventure</t>
+          <t>western</t>
         </is>
       </c>
       <c r="BM1" s="1" t="inlineStr">
-        <is>
-          <t>romantic</t>
-        </is>
-      </c>
-      <c r="BN1" s="1" t="inlineStr">
         <is>
           <t>sci-fi</t>
         </is>
       </c>
+      <c r="BN1" s="1" t="inlineStr">
+        <is>
+          <t>war</t>
+        </is>
+      </c>
       <c r="BO1" s="1" t="inlineStr">
         <is>
-          <t>animation</t>
+          <t>documentary</t>
         </is>
       </c>
       <c r="BP1" s="1" t="inlineStr">
         <is>
-          <t>family</t>
+          <t>mystery</t>
         </is>
       </c>
       <c r="BQ1" s="1" t="inlineStr">
         <is>
-          <t>mystery</t>
+          <t>horror</t>
         </is>
       </c>
       <c r="BR1" s="1" t="inlineStr">
@@ -786,125 +786,115 @@
       </c>
       <c r="BS1" s="1" t="inlineStr">
         <is>
-          <t>documentary</t>
+          <t>adventure</t>
         </is>
       </c>
       <c r="BT1" s="1" t="inlineStr">
+        <is>
+          <t>history</t>
+        </is>
+      </c>
+      <c r="BU1" s="1" t="inlineStr">
+        <is>
+          <t>family</t>
+        </is>
+      </c>
+      <c r="BV1" s="1" t="inlineStr">
+        <is>
+          <t>comedy</t>
+        </is>
+      </c>
+      <c r="BW1" s="1" t="inlineStr">
+        <is>
+          <t>thrilled</t>
+        </is>
+      </c>
+      <c r="BX1" s="1" t="inlineStr">
         <is>
           <t>period</t>
         </is>
       </c>
-      <c r="BU1" s="1" t="inlineStr">
+      <c r="BY1" s="1" t="inlineStr">
         <is>
-          <t>war</t>
+          <t>sports</t>
         </is>
       </c>
-      <c r="BV1" s="1" t="inlineStr">
+      <c r="BZ1" s="1" t="inlineStr">
+        <is>
+          <t>romantic</t>
+        </is>
+      </c>
+      <c r="CA1" s="1" t="inlineStr">
         <is>
           <t>biography</t>
         </is>
       </c>
-      <c r="BW1" s="1" t="inlineStr">
-        <is>
-          <t>drama</t>
-        </is>
-      </c>
-      <c r="BX1" s="1" t="inlineStr">
-        <is>
-          <t>fantasy</t>
-        </is>
-      </c>
-      <c r="BY1" s="1" t="inlineStr">
-        <is>
-          <t>action</t>
-        </is>
-      </c>
-      <c r="BZ1" s="1" t="inlineStr">
-        <is>
-          <t>history</t>
-        </is>
-      </c>
-      <c r="CA1" s="1" t="inlineStr">
-        <is>
-          <t>western</t>
-        </is>
-      </c>
       <c r="CB1" s="1" t="inlineStr">
         <is>
-          <t>thrilled</t>
+          <t>animation</t>
         </is>
       </c>
       <c r="CC1" s="1" t="inlineStr">
-        <is>
-          <t>horror</t>
-        </is>
-      </c>
-      <c r="CD1" s="1" t="inlineStr">
-        <is>
-          <t>crime</t>
-        </is>
-      </c>
-      <c r="CE1" s="1" t="inlineStr">
         <is>
           <t>_april</t>
         </is>
       </c>
-      <c r="CF1" s="1" t="inlineStr">
+      <c r="CD1" s="1" t="inlineStr">
         <is>
           <t>_august</t>
         </is>
       </c>
-      <c r="CG1" s="1" t="inlineStr">
+      <c r="CE1" s="1" t="inlineStr">
         <is>
           <t>_december</t>
         </is>
       </c>
-      <c r="CH1" s="1" t="inlineStr">
+      <c r="CF1" s="1" t="inlineStr">
         <is>
           <t>_february</t>
         </is>
       </c>
-      <c r="CI1" s="1" t="inlineStr">
+      <c r="CG1" s="1" t="inlineStr">
         <is>
           <t>_january</t>
         </is>
       </c>
-      <c r="CJ1" s="1" t="inlineStr">
+      <c r="CH1" s="1" t="inlineStr">
         <is>
           <t>_july</t>
         </is>
       </c>
-      <c r="CK1" s="1" t="inlineStr">
+      <c r="CI1" s="1" t="inlineStr">
         <is>
           <t>_june</t>
         </is>
       </c>
-      <c r="CL1" s="1" t="inlineStr">
+      <c r="CJ1" s="1" t="inlineStr">
         <is>
           <t>_march</t>
         </is>
       </c>
-      <c r="CM1" s="1" t="inlineStr">
+      <c r="CK1" s="1" t="inlineStr">
         <is>
           <t>_may</t>
         </is>
       </c>
-      <c r="CN1" s="1" t="inlineStr">
+      <c r="CL1" s="1" t="inlineStr">
         <is>
           <t>_november</t>
         </is>
       </c>
-      <c r="CO1" s="1" t="inlineStr">
+      <c r="CM1" s="1" t="inlineStr">
         <is>
           <t>_october</t>
         </is>
       </c>
-      <c r="CP1" s="1" t="inlineStr">
+      <c r="CN1" s="1" t="inlineStr">
         <is>
           <t>_september</t>
         </is>
       </c>
-      <c r="CQ1" s="1" t="inlineStr">
+      <c r="CO1" s="1" t="inlineStr">
         <is>
           <t>Predicted_Oscar_Winners</t>
         </is>
@@ -1092,7 +1082,7 @@
         <v>0</v>
       </c>
       <c r="BI2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ2" t="n">
         <v>0</v>
@@ -1140,7 +1130,7 @@
         <v>0</v>
       </c>
       <c r="BY2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ2" t="n">
         <v>0</v>
@@ -1182,19 +1172,13 @@
         <v>0</v>
       </c>
       <c r="CM2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CN2" t="n">
         <v>0</v>
       </c>
       <c r="CO2" t="n">
         <v>1</v>
-      </c>
-      <c r="CP2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ2" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -1400,7 +1384,7 @@
         <v>0</v>
       </c>
       <c r="BP3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ3" t="n">
         <v>0</v>
@@ -1415,7 +1399,7 @@
         <v>0</v>
       </c>
       <c r="BU3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BV3" t="n">
         <v>0</v>
@@ -1469,19 +1453,13 @@
         <v>0</v>
       </c>
       <c r="CM3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CN3" t="n">
         <v>0</v>
       </c>
       <c r="CO3" t="n">
         <v>1</v>
-      </c>
-      <c r="CP3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ3" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -1672,7 +1650,7 @@
         <v>0</v>
       </c>
       <c r="BK4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL4" t="n">
         <v>0</v>
@@ -1705,7 +1683,7 @@
         <v>0</v>
       </c>
       <c r="BV4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BW4" t="n">
         <v>0</v>
@@ -1744,13 +1722,13 @@
         <v>0</v>
       </c>
       <c r="CI4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CJ4" t="n">
         <v>0</v>
       </c>
       <c r="CK4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CL4" t="n">
         <v>0</v>
@@ -1762,13 +1740,7 @@
         <v>0</v>
       </c>
       <c r="CO4" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP4" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -1959,7 +1931,7 @@
         <v>0</v>
       </c>
       <c r="BK5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL5" t="n">
         <v>0</v>
@@ -1998,7 +1970,7 @@
         <v>0</v>
       </c>
       <c r="BX5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY5" t="n">
         <v>0</v>
@@ -2031,13 +2003,13 @@
         <v>0</v>
       </c>
       <c r="CI5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CJ5" t="n">
         <v>0</v>
       </c>
       <c r="CK5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CL5" t="n">
         <v>0</v>
@@ -2049,13 +2021,7 @@
         <v>0</v>
       </c>
       <c r="CO5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -2246,7 +2212,7 @@
         <v>0</v>
       </c>
       <c r="BK6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL6" t="n">
         <v>0</v>
@@ -2279,7 +2245,7 @@
         <v>0</v>
       </c>
       <c r="BV6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BW6" t="n">
         <v>0</v>
@@ -2324,25 +2290,19 @@
         <v>0</v>
       </c>
       <c r="CK6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CL6" t="n">
         <v>0</v>
       </c>
       <c r="CM6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CN6" t="n">
         <v>0</v>
       </c>
       <c r="CO6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -2524,7 +2484,7 @@
         <v>0</v>
       </c>
       <c r="BH7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI7" t="n">
         <v>0</v>
@@ -2566,13 +2526,13 @@
         <v>0</v>
       </c>
       <c r="BV7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BW7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY7" t="n">
         <v>0</v>
@@ -2614,22 +2574,16 @@
         <v>0</v>
       </c>
       <c r="CL7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CM7" t="n">
         <v>0</v>
       </c>
       <c r="CN7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CO7" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP7" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -2820,7 +2774,7 @@
         <v>0</v>
       </c>
       <c r="BK8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL8" t="n">
         <v>0</v>
@@ -2838,7 +2792,7 @@
         <v>0</v>
       </c>
       <c r="BQ8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BR8" t="n">
         <v>0</v>
@@ -2853,7 +2807,7 @@
         <v>0</v>
       </c>
       <c r="BV8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BW8" t="n">
         <v>0</v>
@@ -2874,7 +2828,7 @@
         <v>0</v>
       </c>
       <c r="CC8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD8" t="n">
         <v>0</v>
@@ -2892,13 +2846,13 @@
         <v>0</v>
       </c>
       <c r="CI8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CJ8" t="n">
         <v>0</v>
       </c>
       <c r="CK8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CL8" t="n">
         <v>0</v>
@@ -2910,13 +2864,7 @@
         <v>0</v>
       </c>
       <c r="CO8" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP8" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -3110,13 +3058,13 @@
         <v>0</v>
       </c>
       <c r="BL9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO9" t="n">
         <v>0</v>
@@ -3131,7 +3079,7 @@
         <v>0</v>
       </c>
       <c r="BS9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BT9" t="n">
         <v>0</v>
@@ -3182,13 +3130,13 @@
         <v>0</v>
       </c>
       <c r="CJ9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CK9" t="n">
         <v>0</v>
       </c>
       <c r="CL9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CM9" t="n">
         <v>0</v>
@@ -3197,13 +3145,7 @@
         <v>0</v>
       </c>
       <c r="CO9" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP9" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -3394,7 +3336,7 @@
         <v>0</v>
       </c>
       <c r="BK10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL10" t="n">
         <v>0</v>
@@ -3427,7 +3369,7 @@
         <v>0</v>
       </c>
       <c r="BV10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BW10" t="n">
         <v>0</v>
@@ -3469,13 +3411,13 @@
         <v>0</v>
       </c>
       <c r="CJ10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CK10" t="n">
         <v>0</v>
       </c>
       <c r="CL10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CM10" t="n">
         <v>0</v>
@@ -3484,13 +3426,7 @@
         <v>0</v>
       </c>
       <c r="CO10" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP10" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -3684,7 +3620,7 @@
         <v>0</v>
       </c>
       <c r="BL11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM11" t="n">
         <v>0</v>
@@ -3705,7 +3641,7 @@
         <v>0</v>
       </c>
       <c r="BS11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BT11" t="n">
         <v>0</v>
@@ -3753,13 +3689,13 @@
         <v>0</v>
       </c>
       <c r="CI11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CJ11" t="n">
         <v>0</v>
       </c>
       <c r="CK11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CL11" t="n">
         <v>0</v>
@@ -3771,13 +3707,7 @@
         <v>0</v>
       </c>
       <c r="CO11" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP11" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -3968,7 +3898,7 @@
         <v>0</v>
       </c>
       <c r="BK12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL12" t="n">
         <v>0</v>
@@ -4007,7 +3937,7 @@
         <v>0</v>
       </c>
       <c r="BX12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY12" t="n">
         <v>0</v>
@@ -4055,16 +3985,10 @@
         <v>0</v>
       </c>
       <c r="CN12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CO12" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP12" t="n">
-        <v>1</v>
-      </c>
-      <c r="CQ12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -4282,7 +4206,7 @@
         <v>0</v>
       </c>
       <c r="BT13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BU13" t="n">
         <v>0</v>
@@ -4300,7 +4224,7 @@
         <v>0</v>
       </c>
       <c r="BZ13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA13" t="n">
         <v>0</v>
@@ -4327,13 +4251,13 @@
         <v>0</v>
       </c>
       <c r="CI13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CJ13" t="n">
         <v>0</v>
       </c>
       <c r="CK13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CL13" t="n">
         <v>0</v>
@@ -4345,13 +4269,7 @@
         <v>0</v>
       </c>
       <c r="CO13" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP13" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -4533,7 +4451,7 @@
         <v>0</v>
       </c>
       <c r="BH14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI14" t="n">
         <v>0</v>
@@ -4578,7 +4496,7 @@
         <v>0</v>
       </c>
       <c r="BW14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX14" t="n">
         <v>0</v>
@@ -4614,13 +4532,13 @@
         <v>0</v>
       </c>
       <c r="CI14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CJ14" t="n">
         <v>0</v>
       </c>
       <c r="CK14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CL14" t="n">
         <v>0</v>
@@ -4632,13 +4550,7 @@
         <v>0</v>
       </c>
       <c r="CO14" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP14" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -4829,7 +4741,7 @@
         <v>0</v>
       </c>
       <c r="BK15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL15" t="n">
         <v>0</v>
@@ -4862,7 +4774,7 @@
         <v>0</v>
       </c>
       <c r="BV15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BW15" t="n">
         <v>0</v>
@@ -4913,19 +4825,13 @@
         <v>0</v>
       </c>
       <c r="CM15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CN15" t="n">
         <v>0</v>
       </c>
       <c r="CO15" t="n">
         <v>1</v>
-      </c>
-      <c r="CP15" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ15" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -5122,10 +5028,10 @@
         <v>0</v>
       </c>
       <c r="BM16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO16" t="n">
         <v>0</v>
@@ -5134,7 +5040,7 @@
         <v>0</v>
       </c>
       <c r="BQ16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BR16" t="n">
         <v>0</v>
@@ -5170,7 +5076,7 @@
         <v>0</v>
       </c>
       <c r="CC16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD16" t="n">
         <v>0</v>
@@ -5197,22 +5103,16 @@
         <v>0</v>
       </c>
       <c r="CL16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CM16" t="n">
         <v>0</v>
       </c>
       <c r="CN16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CO16" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP16" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -5397,7 +5297,7 @@
         <v>0</v>
       </c>
       <c r="BI17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ17" t="n">
         <v>0</v>
@@ -5445,7 +5345,7 @@
         <v>0</v>
       </c>
       <c r="BY17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ17" t="n">
         <v>0</v>
@@ -5472,13 +5372,13 @@
         <v>0</v>
       </c>
       <c r="CH17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CI17" t="n">
         <v>0</v>
       </c>
       <c r="CJ17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CK17" t="n">
         <v>0</v>
@@ -5493,13 +5393,7 @@
         <v>0</v>
       </c>
       <c r="CO17" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP17" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -5693,7 +5587,7 @@
         <v>0</v>
       </c>
       <c r="BL18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM18" t="n">
         <v>0</v>
@@ -5714,7 +5608,7 @@
         <v>0</v>
       </c>
       <c r="BS18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BT18" t="n">
         <v>0</v>
@@ -5753,13 +5647,13 @@
         <v>0</v>
       </c>
       <c r="CF18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CG18" t="n">
         <v>0</v>
       </c>
       <c r="CH18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI18" t="n">
         <v>0</v>
@@ -5780,13 +5674,7 @@
         <v>0</v>
       </c>
       <c r="CO18" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP18" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -6040,13 +5928,13 @@
         <v>0</v>
       </c>
       <c r="CF19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CG19" t="n">
         <v>0</v>
       </c>
       <c r="CH19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI19" t="n">
         <v>0</v>
@@ -6067,13 +5955,7 @@
         <v>0</v>
       </c>
       <c r="CO19" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP19" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -6255,7 +6137,7 @@
         <v>0</v>
       </c>
       <c r="BH20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI20" t="n">
         <v>0</v>
@@ -6300,7 +6182,7 @@
         <v>0</v>
       </c>
       <c r="BW20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX20" t="n">
         <v>0</v>
@@ -6324,13 +6206,13 @@
         <v>0</v>
       </c>
       <c r="CE20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CF20" t="n">
         <v>0</v>
       </c>
       <c r="CG20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH20" t="n">
         <v>0</v>
@@ -6354,13 +6236,7 @@
         <v>0</v>
       </c>
       <c r="CO20" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP20" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -6563,7 +6439,7 @@
         <v>0</v>
       </c>
       <c r="BO21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP21" t="n">
         <v>0</v>
@@ -6602,7 +6478,7 @@
         <v>0</v>
       </c>
       <c r="CB21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CC21" t="n">
         <v>0</v>
@@ -6632,22 +6508,16 @@
         <v>0</v>
       </c>
       <c r="CL21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CM21" t="n">
         <v>0</v>
       </c>
       <c r="CN21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CO21" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP21" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -6919,21 +6789,15 @@
         <v>0</v>
       </c>
       <c r="CL22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CM22" t="n">
         <v>0</v>
       </c>
       <c r="CN22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CO22" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP22" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ22" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7116,7 +6980,7 @@
         <v>0</v>
       </c>
       <c r="BH23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI23" t="n">
         <v>0</v>
@@ -7161,7 +7025,7 @@
         <v>0</v>
       </c>
       <c r="BW23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX23" t="n">
         <v>0</v>
@@ -7200,13 +7064,13 @@
         <v>0</v>
       </c>
       <c r="CJ23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CK23" t="n">
         <v>0</v>
       </c>
       <c r="CL23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CM23" t="n">
         <v>0</v>
@@ -7215,13 +7079,7 @@
         <v>0</v>
       </c>
       <c r="CO23" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP23" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
@@ -7427,10 +7285,10 @@
         <v>0</v>
       </c>
       <c r="BP24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BQ24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR24" t="n">
         <v>1</v>
@@ -7448,7 +7306,7 @@
         <v>0</v>
       </c>
       <c r="BW24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX24" t="n">
         <v>0</v>
@@ -7463,7 +7321,7 @@
         <v>0</v>
       </c>
       <c r="CB24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC24" t="n">
         <v>0</v>
@@ -7487,13 +7345,13 @@
         <v>0</v>
       </c>
       <c r="CJ24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CK24" t="n">
         <v>0</v>
       </c>
       <c r="CL24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CM24" t="n">
         <v>0</v>
@@ -7502,13 +7360,7 @@
         <v>0</v>
       </c>
       <c r="CO24" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP24" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -7780,22 +7632,16 @@
         <v>0</v>
       </c>
       <c r="CL25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CM25" t="n">
         <v>0</v>
       </c>
       <c r="CN25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CO25" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP25" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -8001,10 +7847,10 @@
         <v>0</v>
       </c>
       <c r="BP26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BQ26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR26" t="n">
         <v>0</v>
@@ -8022,7 +7868,7 @@
         <v>0</v>
       </c>
       <c r="BW26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX26" t="n">
         <v>0</v>
@@ -8037,7 +7883,7 @@
         <v>0</v>
       </c>
       <c r="CB26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC26" t="n">
         <v>0</v>
@@ -8067,22 +7913,16 @@
         <v>0</v>
       </c>
       <c r="CL26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CM26" t="n">
         <v>0</v>
       </c>
       <c r="CN26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CO26" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP26" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -8333,13 +8173,13 @@
         <v>0</v>
       </c>
       <c r="CE27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CF27" t="n">
         <v>0</v>
       </c>
       <c r="CG27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH27" t="n">
         <v>0</v>
@@ -8363,13 +8203,7 @@
         <v>0</v>
       </c>
       <c r="CO27" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP27" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -8563,7 +8397,7 @@
         <v>0</v>
       </c>
       <c r="BL28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM28" t="n">
         <v>0</v>
@@ -8584,7 +8418,7 @@
         <v>0</v>
       </c>
       <c r="BS28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BT28" t="n">
         <v>0</v>
@@ -8617,13 +8451,13 @@
         <v>0</v>
       </c>
       <c r="CD28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CE28" t="n">
         <v>0</v>
       </c>
       <c r="CF28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG28" t="n">
         <v>0</v>
@@ -8650,13 +8484,7 @@
         <v>0</v>
       </c>
       <c r="CO28" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP28" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
@@ -8847,7 +8675,7 @@
         <v>0</v>
       </c>
       <c r="BK29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL29" t="n">
         <v>0</v>
@@ -8880,7 +8708,7 @@
         <v>0</v>
       </c>
       <c r="BV29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BW29" t="n">
         <v>0</v>
@@ -8919,13 +8747,13 @@
         <v>0</v>
       </c>
       <c r="CI29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CJ29" t="n">
         <v>0</v>
       </c>
       <c r="CK29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CL29" t="n">
         <v>0</v>
@@ -8937,13 +8765,7 @@
         <v>0</v>
       </c>
       <c r="CO29" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP29" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -9149,7 +8971,7 @@
         <v>0</v>
       </c>
       <c r="BP30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ30" t="n">
         <v>0</v>
@@ -9164,16 +8986,16 @@
         <v>0</v>
       </c>
       <c r="BU30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BV30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BW30" t="n">
         <v>0</v>
       </c>
       <c r="BX30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY30" t="n">
         <v>0</v>
@@ -9206,13 +9028,13 @@
         <v>0</v>
       </c>
       <c r="CI30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CJ30" t="n">
         <v>0</v>
       </c>
       <c r="CK30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CL30" t="n">
         <v>0</v>
@@ -9224,13 +9046,7 @@
         <v>0</v>
       </c>
       <c r="CO30" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP30" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
@@ -9412,7 +9228,7 @@
         <v>0</v>
       </c>
       <c r="BH31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI31" t="n">
         <v>0</v>
@@ -9436,10 +9252,10 @@
         <v>0</v>
       </c>
       <c r="BP31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BQ31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR31" t="n">
         <v>0</v>
@@ -9448,7 +9264,7 @@
         <v>0</v>
       </c>
       <c r="BT31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BU31" t="n">
         <v>0</v>
@@ -9466,13 +9282,13 @@
         <v>0</v>
       </c>
       <c r="BZ31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA31" t="n">
         <v>0</v>
       </c>
       <c r="CB31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC31" t="n">
         <v>0</v>
@@ -9493,13 +9309,13 @@
         <v>0</v>
       </c>
       <c r="CI31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CJ31" t="n">
         <v>0</v>
       </c>
       <c r="CK31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CL31" t="n">
         <v>0</v>
@@ -9511,13 +9327,7 @@
         <v>0</v>
       </c>
       <c r="CO31" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP31" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -9699,7 +9509,7 @@
         <v>0</v>
       </c>
       <c r="BH32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI32" t="n">
         <v>0</v>
@@ -9744,7 +9554,7 @@
         <v>0</v>
       </c>
       <c r="BW32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX32" t="n">
         <v>0</v>
@@ -9768,13 +9578,13 @@
         <v>0</v>
       </c>
       <c r="CE32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CF32" t="n">
         <v>0</v>
       </c>
       <c r="CG32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH32" t="n">
         <v>0</v>
@@ -9798,13 +9608,7 @@
         <v>0</v>
       </c>
       <c r="CO32" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP32" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -9986,7 +9790,7 @@
         <v>0</v>
       </c>
       <c r="BH33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI33" t="n">
         <v>0</v>
@@ -10031,7 +9835,7 @@
         <v>0</v>
       </c>
       <c r="BW33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX33" t="n">
         <v>0</v>
@@ -10079,19 +9883,13 @@
         <v>0</v>
       </c>
       <c r="CM33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CN33" t="n">
         <v>0</v>
       </c>
       <c r="CO33" t="n">
         <v>1</v>
-      </c>
-      <c r="CP33" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ33" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -10351,13 +10149,13 @@
         <v>0</v>
       </c>
       <c r="CH34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CI34" t="n">
         <v>0</v>
       </c>
       <c r="CJ34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CK34" t="n">
         <v>0</v>
@@ -10372,13 +10170,7 @@
         <v>0</v>
       </c>
       <c r="CO34" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP34" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
@@ -10569,7 +10361,7 @@
         <v>0</v>
       </c>
       <c r="BK35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL35" t="n">
         <v>0</v>
@@ -10602,7 +10394,7 @@
         <v>0</v>
       </c>
       <c r="BV35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BW35" t="n">
         <v>0</v>
@@ -10650,22 +10442,16 @@
         <v>0</v>
       </c>
       <c r="CL35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CM35" t="n">
         <v>0</v>
       </c>
       <c r="CN35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CO35" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP35" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -10874,7 +10660,7 @@
         <v>0</v>
       </c>
       <c r="BQ36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BR36" t="n">
         <v>0</v>
@@ -10916,7 +10702,7 @@
         <v>0</v>
       </c>
       <c r="CE36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF36" t="n">
         <v>0</v>
@@ -10946,13 +10732,7 @@
         <v>0</v>
       </c>
       <c r="CO36" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP36" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
@@ -11143,7 +10923,7 @@
         <v>0</v>
       </c>
       <c r="BK37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL37" t="n">
         <v>0</v>
@@ -11176,7 +10956,7 @@
         <v>0</v>
       </c>
       <c r="BV37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BW37" t="n">
         <v>0</v>
@@ -11221,25 +11001,19 @@
         <v>0</v>
       </c>
       <c r="CK37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CL37" t="n">
         <v>0</v>
       </c>
       <c r="CM37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CN37" t="n">
         <v>0</v>
       </c>
       <c r="CO37" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP37" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -11421,7 +11195,7 @@
         <v>0</v>
       </c>
       <c r="BH38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI38" t="n">
         <v>0</v>
@@ -11466,7 +11240,7 @@
         <v>0</v>
       </c>
       <c r="BW38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX38" t="n">
         <v>0</v>
@@ -11487,13 +11261,13 @@
         <v>0</v>
       </c>
       <c r="CD38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CE38" t="n">
         <v>0</v>
       </c>
       <c r="CF38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG38" t="n">
         <v>0</v>
@@ -11520,13 +11294,7 @@
         <v>0</v>
       </c>
       <c r="CO38" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP38" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
@@ -11708,7 +11476,7 @@
         <v>0</v>
       </c>
       <c r="BH39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI39" t="n">
         <v>0</v>
@@ -11753,7 +11521,7 @@
         <v>0</v>
       </c>
       <c r="BW39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX39" t="n">
         <v>0</v>
@@ -11774,13 +11542,13 @@
         <v>0</v>
       </c>
       <c r="CD39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CE39" t="n">
         <v>0</v>
       </c>
       <c r="CF39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG39" t="n">
         <v>0</v>
@@ -11807,12 +11575,6 @@
         <v>0</v>
       </c>
       <c r="CO39" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP39" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ39" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11998,7 +11760,7 @@
         <v>0</v>
       </c>
       <c r="BI40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ40" t="n">
         <v>0</v>
@@ -12046,7 +11808,7 @@
         <v>0</v>
       </c>
       <c r="BY40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ40" t="n">
         <v>0</v>
@@ -12082,25 +11844,19 @@
         <v>0</v>
       </c>
       <c r="CK40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CL40" t="n">
         <v>0</v>
       </c>
       <c r="CM40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CN40" t="n">
         <v>0</v>
       </c>
       <c r="CO40" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP40" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
@@ -12327,7 +12083,7 @@
         <v>0</v>
       </c>
       <c r="BW41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX41" t="n">
         <v>0</v>
@@ -12342,19 +12098,19 @@
         <v>0</v>
       </c>
       <c r="CB41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC41" t="n">
         <v>0</v>
       </c>
       <c r="CD41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CE41" t="n">
         <v>0</v>
       </c>
       <c r="CF41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG41" t="n">
         <v>0</v>
@@ -12381,13 +12137,7 @@
         <v>0</v>
       </c>
       <c r="CO41" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP41" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -12572,7 +12322,7 @@
         <v>0</v>
       </c>
       <c r="BI42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ42" t="n">
         <v>0</v>
@@ -12620,7 +12370,7 @@
         <v>0</v>
       </c>
       <c r="BY42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ42" t="n">
         <v>0</v>
@@ -12659,22 +12409,16 @@
         <v>0</v>
       </c>
       <c r="CL42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CM42" t="n">
         <v>0</v>
       </c>
       <c r="CN42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CO42" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP42" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
@@ -12925,13 +12669,13 @@
         <v>0</v>
       </c>
       <c r="CE43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CF43" t="n">
         <v>0</v>
       </c>
       <c r="CG43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH43" t="n">
         <v>0</v>
@@ -12955,13 +12699,7 @@
         <v>0</v>
       </c>
       <c r="CO43" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP43" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44">
@@ -13212,13 +12950,13 @@
         <v>0</v>
       </c>
       <c r="CE44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CF44" t="n">
         <v>0</v>
       </c>
       <c r="CG44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH44" t="n">
         <v>0</v>
@@ -13242,13 +12980,7 @@
         <v>0</v>
       </c>
       <c r="CO44" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP44" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -13439,7 +13171,7 @@
         <v>0</v>
       </c>
       <c r="BK45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL45" t="n">
         <v>0</v>
@@ -13472,7 +13204,7 @@
         <v>0</v>
       </c>
       <c r="BV45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BW45" t="n">
         <v>0</v>
@@ -13520,22 +13252,16 @@
         <v>0</v>
       </c>
       <c r="CL45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CM45" t="n">
         <v>0</v>
       </c>
       <c r="CN45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CO45" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP45" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46">
@@ -13729,7 +13455,7 @@
         <v>0</v>
       </c>
       <c r="BL46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM46" t="n">
         <v>0</v>
@@ -13750,7 +13476,7 @@
         <v>0</v>
       </c>
       <c r="BS46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BT46" t="n">
         <v>0</v>
@@ -13792,13 +13518,13 @@
         <v>0</v>
       </c>
       <c r="CG46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CH46" t="n">
         <v>0</v>
       </c>
       <c r="CI46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ46" t="n">
         <v>0</v>
@@ -13816,13 +13542,7 @@
         <v>0</v>
       </c>
       <c r="CO46" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP46" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
@@ -14004,7 +13724,7 @@
         <v>0</v>
       </c>
       <c r="BH47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI47" t="n">
         <v>0</v>
@@ -14049,7 +13769,7 @@
         <v>0</v>
       </c>
       <c r="BW47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX47" t="n">
         <v>0</v>
@@ -14082,13 +13802,13 @@
         <v>0</v>
       </c>
       <c r="CH47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CI47" t="n">
         <v>0</v>
       </c>
       <c r="CJ47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CK47" t="n">
         <v>0</v>
@@ -14103,13 +13823,7 @@
         <v>0</v>
       </c>
       <c r="CO47" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP47" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48">
@@ -14318,7 +14032,7 @@
         <v>0</v>
       </c>
       <c r="BQ48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BR48" t="n">
         <v>0</v>
@@ -14354,7 +14068,7 @@
         <v>0</v>
       </c>
       <c r="CC48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD48" t="n">
         <v>0</v>
@@ -14387,16 +14101,10 @@
         <v>0</v>
       </c>
       <c r="CN48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CO48" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP48" t="n">
-        <v>1</v>
-      </c>
-      <c r="CQ48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
@@ -14584,7 +14292,7 @@
         <v>0</v>
       </c>
       <c r="BJ49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK49" t="n">
         <v>0</v>
@@ -14602,10 +14310,10 @@
         <v>0</v>
       </c>
       <c r="BP49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BQ49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR49" t="n">
         <v>0</v>
@@ -14644,7 +14352,7 @@
         <v>0</v>
       </c>
       <c r="CD49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE49" t="n">
         <v>0</v>
@@ -14674,16 +14382,10 @@
         <v>0</v>
       </c>
       <c r="CN49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CO49" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP49" t="n">
-        <v>1</v>
-      </c>
-      <c r="CQ49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50">
@@ -14868,7 +14570,7 @@
         <v>0</v>
       </c>
       <c r="BI50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ50" t="n">
         <v>0</v>
@@ -14916,7 +14618,7 @@
         <v>0</v>
       </c>
       <c r="BY50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ50" t="n">
         <v>0</v>
@@ -14928,13 +14630,13 @@
         <v>0</v>
       </c>
       <c r="CC50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CD50" t="n">
         <v>0</v>
       </c>
       <c r="CE50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF50" t="n">
         <v>0</v>
@@ -14964,13 +14666,7 @@
         <v>0</v>
       </c>
       <c r="CO50" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP50" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51">
@@ -15155,16 +14851,16 @@
         <v>0</v>
       </c>
       <c r="BI51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ51" t="n">
         <v>0</v>
       </c>
       <c r="BK51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM51" t="n">
         <v>0</v>
@@ -15185,7 +14881,7 @@
         <v>0</v>
       </c>
       <c r="BS51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BT51" t="n">
         <v>0</v>
@@ -15194,7 +14890,7 @@
         <v>0</v>
       </c>
       <c r="BV51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BW51" t="n">
         <v>0</v>
@@ -15203,7 +14899,7 @@
         <v>0</v>
       </c>
       <c r="BY51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ51" t="n">
         <v>0</v>
@@ -15215,13 +14911,13 @@
         <v>0</v>
       </c>
       <c r="CC51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CD51" t="n">
         <v>0</v>
       </c>
       <c r="CE51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF51" t="n">
         <v>0</v>
@@ -15251,13 +14947,7 @@
         <v>0</v>
       </c>
       <c r="CO51" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP51" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>